<commit_message>
CNN+LSTM run sgd on cluster
</commit_message>
<xml_diff>
--- a/models/Results.xlsx
+++ b/models/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Q4\ACVPR\project_19\advanced_computer_vision\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD71D45-3CE3-4FA2-86AA-B3FFDAB6B332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E3BD4D-0565-4650-9149-B05B860F31A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2710EA61-769D-4270-8F08-7D185850AFBB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="22">
   <si>
     <t>Model architecture</t>
   </si>
@@ -79,15 +79,6 @@
     <t># epochs</t>
   </si>
   <si>
-    <t>310min</t>
-  </si>
-  <si>
-    <t>310s per epoch</t>
-  </si>
-  <si>
-    <t>63s</t>
-  </si>
-  <si>
     <t>83min</t>
   </si>
   <si>
@@ -100,10 +91,16 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Run on GTX 1060 laptop 6GB, Intel Core i5 8350H, 16GB RAM</t>
-  </si>
-  <si>
     <t>Run on Tesla T4 24GB</t>
+  </si>
+  <si>
+    <t>210min</t>
+  </si>
+  <si>
+    <t>210s per epoch</t>
+  </si>
+  <si>
+    <t>52.1s</t>
   </si>
 </sst>
 </file>
@@ -150,37 +147,17 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -514,7 +491,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,11 +524,11 @@
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -564,7 +541,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E2">
         <v>24</v>
@@ -575,11 +552,11 @@
       <c r="G2">
         <v>0.2</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -592,7 +569,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3">
         <v>71.599999999999994</v>
@@ -600,9 +577,9 @@
       <c r="G3">
         <v>1.46</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -615,16 +592,16 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>72.099999999999994</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="6" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -635,22 +612,22 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>60</v>
       </c>
       <c r="F6">
-        <v>80.099999999999994</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="G6">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -663,17 +640,17 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F7">
-        <v>63.7</v>
+        <v>69.8</v>
       </c>
       <c r="G7">
-        <v>1.22</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+        <v>0.9</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -686,14 +663,14 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F8">
-        <v>68</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+        <v>71.2</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -834,14 +811,14 @@
     <mergeCell ref="H6:J8"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C4 C6:C8 C10:C12 C14:C16 C18:C20 C22:C24">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="SGD">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="SGD">
       <formula>NOT(ISERROR(SEARCH("SGD",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Adam">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Adam">
       <formula>NOT(ISERROR(SEARCH("Adam",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8 F4 F12 F16 F20 F24">
+  <conditionalFormatting sqref="F4 F8 F12 F16 F20 F24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
updated results for sgd cnn+lstm
</commit_message>
<xml_diff>
--- a/models/Results.xlsx
+++ b/models/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>Type</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>28.3s</t>
+  </si>
+  <si>
+    <t>63min</t>
+  </si>
+  <si>
+    <t>127s per epoch</t>
+  </si>
+  <si>
+    <t>29.4s</t>
   </si>
   <si>
     <t>ConvLSTM</t>
@@ -120,7 +129,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +139,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -169,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -195,17 +210,20 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -550,15 +568,15 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="13" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="17" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="17" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="17" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="15" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="18" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="18" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="18" width="9.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -593,7 +611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="39.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -668,18 +686,18 @@
       <c r="J4" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="11"/>
+      <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="39.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="46.5">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -754,18 +772,18 @@
       <c r="J8" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="46.5">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -781,7 +799,7 @@
       <c r="E10" s="9">
         <v>60</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <v>99.09</v>
       </c>
       <c r="G10" s="10">
@@ -807,7 +825,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <v>55.81</v>
       </c>
       <c r="G11" s="10">
@@ -831,7 +849,7 @@
         <v>26</v>
       </c>
       <c r="E12" s="9"/>
-      <c r="F12" s="11">
+      <c r="F12" s="10">
         <v>52.12</v>
       </c>
       <c r="G12" s="10"/>
@@ -840,12 +858,12 @@
       <c r="J12" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
@@ -861,11 +879,21 @@
       <c r="C14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="12"/>
+      <c r="D14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="9">
+        <v>30</v>
+      </c>
+      <c r="F14" s="10">
+        <v>75.63</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0.6765</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
     </row>
@@ -879,10 +907,16 @@
       <c r="C15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
+      <c r="F15" s="10">
+        <v>48.84</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1.5525</v>
+      </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -897,38 +931,42 @@
       <c r="C16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="11"/>
+      <c r="F16" s="10">
+        <v>50.2</v>
+      </c>
       <c r="G16" s="10"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="39.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="46.5">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E18" s="6">
         <v>16</v>
@@ -950,13 +988,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="7">
@@ -974,13 +1012,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="7">
@@ -992,29 +1030,29 @@
       <c r="J20" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="11"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="39.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="46.5">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E22" s="6">
         <v>17</v>
@@ -1036,13 +1074,13 @@
         <v>15</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="7">
@@ -1060,13 +1098,13 @@
         <v>17</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="7">

</xml_diff>